<commit_message>
updt alert ref; logic if stor/ANF not used
</commit_message>
<xml_diff>
--- a/references/alerts.xlsx
+++ b/references/alerts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcore.NORTHAMERICA\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepo\AVDAlerts\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD39416-5E94-4848-8DB3-18E54F903E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693BDB13-328A-4072-AE08-A8087693200A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="8085" windowWidth="29040" windowHeight="15720" xr2:uid="{1747E9F3-8C51-4656-9796-47111650C799}"/>
   </bookViews>
@@ -164,21 +164,9 @@
     <t>AVD-Storage-Azure Files Availability-below 99%-{storacctname}</t>
   </si>
   <si>
-    <t>Storage for the follow Azure NetApp volume is critically low (MSIX app packages)</t>
-  </si>
-  <si>
     <t>Verify sufficient storage is available and expand when/where needed</t>
   </si>
   <si>
-    <t>Storage for the follow Azure Files share is critically low (User Profiles/FSLogix)</t>
-  </si>
-  <si>
-    <t>Storage for the follow Azure NetApp volume is moderately low (MSIX app packages)</t>
-  </si>
-  <si>
-    <t>Storage for the follow Azure Files share is moderately low (User Profiles/FSLogix)</t>
-  </si>
-  <si>
     <t>verify automation for storage is  expanding and functional</t>
   </si>
   <si>
@@ -255,6 +243,18 @@
   </si>
   <si>
     <t>Confirm user and storage are in the same region and/or investigate.  Identify sources of latency.</t>
+  </si>
+  <si>
+    <t>Storage for the follow Azure NetApp volume is critically low</t>
+  </si>
+  <si>
+    <t>Storage for the follow Azure Files share is critically low</t>
+  </si>
+  <si>
+    <t>Storage for the follow Azure Files share is moderately low</t>
+  </si>
+  <si>
+    <t>Storage for the follow Azure NetApp volume is moderately low</t>
   </si>
 </sst>
 </file>
@@ -810,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4D25CA4-DB62-4CFC-AE65-12A371E961DC}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -864,7 +864,7 @@
         <v>40</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -885,13 +885,13 @@
         <v>9</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="8"/>
       <c r="B4" s="12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C4" s="13">
         <v>1</v>
@@ -903,10 +903,10 @@
         <v>10</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="24.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -927,7 +927,7 @@
         <v>38</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -948,7 +948,7 @@
         <v>39</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -977,10 +977,10 @@
         <v>10</v>
       </c>
       <c r="F8" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -998,10 +998,10 @@
         <v>10</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -1019,10 +1019,10 @@
         <v>10</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -1040,10 +1040,10 @@
         <v>10</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -1061,10 +1061,10 @@
         <v>13</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -1082,10 +1082,10 @@
         <v>13</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -1103,10 +1103,10 @@
         <v>7</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1135,10 +1135,10 @@
         <v>7</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -1156,10 +1156,10 @@
         <v>7</v>
       </c>
       <c r="F17" s="28" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G17" s="28" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1177,10 +1177,10 @@
         <v>7</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -1198,10 +1198,10 @@
         <v>7</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G19" s="28" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -1219,10 +1219,10 @@
         <v>7</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -1240,10 +1240,10 @@
         <v>7</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G21" s="28" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -1261,10 +1261,10 @@
         <v>13</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -1282,10 +1282,10 @@
         <v>13</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G23" s="28" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
See readme, fslogix event alerts, remove stor LA
</commit_message>
<xml_diff>
--- a/references/alerts.xlsx
+++ b/references/alerts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepo\AVDAlerts\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693BDB13-328A-4072-AE08-A8087693200A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF181BE-B566-4499-9088-FF79CF44D409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="8085" windowWidth="29040" windowHeight="15720" xr2:uid="{1747E9F3-8C51-4656-9796-47111650C799}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{1747E9F3-8C51-4656-9796-47111650C799}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="90">
   <si>
     <t>Alert Name</t>
   </si>
@@ -98,9 +98,6 @@
     <t>AVD-Storage-Low Space on Azure File Share-15% Remaining **</t>
   </si>
   <si>
-    <t>AVD-Storage-Over 200ms Latency for Storage Act-{storacctname}</t>
-  </si>
-  <si>
     <t>AVD-Storage-Possible Throttling Due to High IOPs-{storacctname}</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>AVD-VM-Available Memory Less Than 2GB</t>
   </si>
   <si>
-    <t>AVD-VM-FSLogix Profile Failed (Event Log Indicated Failure)</t>
-  </si>
-  <si>
     <t>AVD-VM-Health Check Failure</t>
   </si>
   <si>
@@ -194,12 +188,6 @@
     <t>Investigate session host memory usage per user and/or memory requirements and adjust if/as needed.  Check user active vs. disconnected status.</t>
   </si>
   <si>
-    <t>Check event logs on VM and FSLogix logs</t>
-  </si>
-  <si>
-    <t>User Profiles Service logged an error</t>
-  </si>
-  <si>
     <t>One or more componets for the AVD serivice has failed</t>
   </si>
   <si>
@@ -255,13 +243,76 @@
   </si>
   <si>
     <t>Storage for the follow Azure NetApp volume is moderately low</t>
+  </si>
+  <si>
+    <t>AVD-Storage-Over 100ms Latency for Storage Act-{storacctname}</t>
+  </si>
+  <si>
+    <t>AVD-Storage-Over 50ms Latency for Storage Act-{storacctname}</t>
+  </si>
+  <si>
+    <t>AVD-Storage-Over 100ms Latency Between Client-Storage-{storacctname}</t>
+  </si>
+  <si>
+    <t>AVD-Storage-Over 50ms Latency Between Client-Storage-{storacctname}</t>
+  </si>
+  <si>
+    <t>AVD-VM-FSLogix Profile Failed (Less Than 2% Free Space)</t>
+  </si>
+  <si>
+    <t>User Profiles Service logged an Event ID 34</t>
+  </si>
+  <si>
+    <t>Expand User's Virtual Profile Disk and/or clean up user profile data.</t>
+  </si>
+  <si>
+    <t>AVD-VM-FSLogix Profile Failed (Less Than 5% Free Space)</t>
+  </si>
+  <si>
+    <t>User Profiles Service logged an Event ID 33</t>
+  </si>
+  <si>
+    <t>AVD-VM-FSLogix Profile Failed due to Network Issue</t>
+  </si>
+  <si>
+    <t>User Profiles Service logged an Event ID 43</t>
+  </si>
+  <si>
+    <t>Verify network communications between the storage and AVD VM</t>
+  </si>
+  <si>
+    <t>AVD-VM-FSLogix Profile Disk Failed to Attach</t>
+  </si>
+  <si>
+    <t>User Profiles Service logged an Event ID 52 or 40</t>
+  </si>
+  <si>
+    <t>Investigate error details for reason</t>
+  </si>
+  <si>
+    <t>AVD-VM-FSLogix Profile Service Disabled</t>
+  </si>
+  <si>
+    <t>User Profile Service Disabled</t>
+  </si>
+  <si>
+    <t>Determine why service was disabled and re-enable / start the FSLogix service</t>
+  </si>
+  <si>
+    <t>AVD-VM-FSLogix Profile Disk Compaction Failed</t>
+  </si>
+  <si>
+    <t>See error details for additional information.</t>
+  </si>
+  <si>
+    <t>User Profile Disk marked for compaction due to additonal white space but failed.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,6 +348,12 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -410,7 +467,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -493,6 +550,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -512,7 +578,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -800,7 +866,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -808,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4D25CA4-DB62-4CFC-AE65-12A371E961DC}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -838,10 +904,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -861,10 +927,10 @@
         <v>7</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -885,13 +951,13 @@
         <v>9</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="8"/>
       <c r="B4" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C4" s="13">
         <v>1</v>
@@ -903,10 +969,10 @@
         <v>10</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="24.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -924,10 +990,10 @@
         <v>10</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -945,10 +1011,10 @@
         <v>13</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -977,10 +1043,10 @@
         <v>10</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -998,10 +1064,10 @@
         <v>10</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -1019,10 +1085,10 @@
         <v>10</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -1040,16 +1106,16 @@
         <v>10</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="19"/>
       <c r="B12" s="12" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="C12" s="13">
         <v>2</v>
@@ -1061,19 +1127,19 @@
         <v>13</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="19"/>
       <c r="B13" s="20" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="C13" s="21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" s="21" t="s">
         <v>16</v>
@@ -1082,16 +1148,16 @@
         <v>13</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="23"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="12" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="C14" s="13">
         <v>1</v>
@@ -1100,226 +1166,395 @@
         <v>16</v>
       </c>
       <c r="E14" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="19"/>
+      <c r="B15" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="21">
+        <v>2</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="19"/>
+      <c r="B16" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="13">
+        <v>2</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="23"/>
+      <c r="B17" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="21">
+        <v>1</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F17" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+    </row>
+    <row r="19" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="6">
+        <v>1</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-    </row>
-    <row r="16" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="6">
-        <v>1</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="7" t="s">
+      <c r="G19" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="25"/>
-      <c r="B17" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="27">
-        <v>2</v>
-      </c>
-      <c r="D17" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="28" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="25"/>
-      <c r="B18" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="13">
-        <v>1</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G18" s="14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="25"/>
-      <c r="B19" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="27">
-        <v>1</v>
-      </c>
-      <c r="D19" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="G19" s="28" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="25"/>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="27">
+        <v>2</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="25"/>
+      <c r="B21" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="13">
+        <v>1</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="25"/>
+      <c r="B22" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="27">
+        <v>2</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="25"/>
+      <c r="B23" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="13">
+        <v>1</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="25"/>
+      <c r="B24" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="27">
+        <v>1</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="25"/>
+      <c r="B25" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="13">
+        <v>1</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="45.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="25"/>
+      <c r="B26" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="27">
+        <v>1</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="G26" s="28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="25"/>
+      <c r="B27" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="34">
+        <v>1</v>
+      </c>
+      <c r="D27" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="G27" s="35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="25"/>
+      <c r="B28" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="27">
+        <v>1</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="G28" s="28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="25"/>
+      <c r="B29" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="34">
+        <v>2</v>
+      </c>
+      <c r="D29" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="G29" s="35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="25"/>
+      <c r="B30" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="13">
-        <v>1</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="14" t="s">
+      <c r="C30" s="27">
+        <v>1</v>
+      </c>
+      <c r="D30" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="G30" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="G20" s="14" t="s">
+    </row>
+    <row r="31" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="29"/>
+      <c r="B31" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="34">
+        <v>2</v>
+      </c>
+      <c r="D31" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="35" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="25"/>
-      <c r="B21" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="27">
-        <v>2</v>
-      </c>
-      <c r="D21" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="G21" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="25"/>
-      <c r="B22" s="12" t="s">
+      <c r="G31" s="35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="13">
-        <v>1</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="29"/>
-      <c r="B23" s="26" t="s">
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="27">
-        <v>2</v>
-      </c>
-      <c r="D23" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="G23" s="28" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="31" t="s">
+      <c r="B34" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="32" t="s">
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B35" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>